<commit_message>
Stopped expressions from showing both min and max if they are the same value, added "send to back button" for when all links are removed between tables
Former-commit-id: 1322cc7d6f3e07ffcf6ad2ec4a8daffcaa4bf683
</commit_message>
<xml_diff>
--- a/QSSD/testing/Perfect1-5 - unrelated.xlsx
+++ b/QSSD/testing/Perfect1-5 - unrelated.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni work\ce301_ramsay_foster_b\QSSD\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FDAE07-273F-492C-8512-A9800F25EE1E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8009746-8B41-4DD2-A793-877A90A54983}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Names" sheetId="1" r:id="rId1"/>
-    <sheet name="Salary" sheetId="2" r:id="rId2"/>
-    <sheet name="Emails" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
+    <sheet name="Salary" sheetId="2" r:id="rId3"/>
+    <sheet name="Emails" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
@@ -188,6 +189,9 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>Age</t>
   </si>
 </sst>
 </file>
@@ -506,7 +510,9 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -648,6 +654,117 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{031A72AE-0639-40D6-AF1B-4B41CFAC0454}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -757,7 +874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -884,11 +1001,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B296F8-2C0C-463A-877C-1A45C5705651}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>